<commit_message>
OW-967,added test cases, debugging
</commit_message>
<xml_diff>
--- a/test/callInfo.xlsx
+++ b/test/callInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="USD" sheetId="1" r:id="rId1"/>
@@ -2914,11 +2914,12 @@
   <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>

</xml_diff>